<commit_message>
TestCase for Profile View Page
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\SQA Projects\Programming Hero\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2938315F-A9A8-4784-A477-B4A6DCB092AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="325" xr2:uid="{F390719A-999E-4BA3-AD96-473CCE2BEAD6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="325"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Product Name</t>
   </si>
@@ -68,9 +62,6 @@
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Developer Name (TL)</t>
   </si>
   <si>
     <t>Test Case Reviewed By</t>
@@ -132,13 +123,85 @@
   </si>
   <si>
     <t>Windows, Android</t>
+  </si>
+  <si>
+    <t>Verify that system redirecting user to valid page or not when user click on 'Login' Button from Welcome page.</t>
+  </si>
+  <si>
+    <t>TC_SP_001</t>
+  </si>
+  <si>
+    <t>TC_SP_002</t>
+  </si>
+  <si>
+    <t>Developer Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that GUI of profile page showing as per requirement or not </t>
+  </si>
+  <si>
+    <t>TC_SP_003</t>
+  </si>
+  <si>
+    <t>Check that  *Profile name , *Profile Photo and other important links like *My Classes, Support, *Notification Icon, Shopping Icon, Diamond icon, Programming Hero Logo  are  Showing or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_004</t>
+  </si>
+  <si>
+    <t>Check that user able to update profile details like Profile photo , Name .</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to see the details (*Name, *Student ID, *View Profile button,  *LeaderBoard, *Students Analytics, Bookmarks, Announcement, *Conceptual sessions, *Logout button ) or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_005</t>
+  </si>
+  <si>
+    <t>TC_SP_006</t>
+  </si>
+  <si>
+    <t>TC_SP_007</t>
+  </si>
+  <si>
+    <t>TC_SP_008</t>
+  </si>
+  <si>
+    <t>TC_SP_009</t>
+  </si>
+  <si>
+    <t>TC_SP_010</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Log out' link.</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Bookmark' button.</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Student Analytics' button.</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Leader Board' button.</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Announcement' button.</t>
+  </si>
+  <si>
+    <t>Check that after click on the profile photo user able to visit the proper page of 'Conceptual Sessions' button.</t>
+  </si>
+  <si>
+    <t>TC_SP_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Cases For 'Profile View Section'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +263,17 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,6 +332,24 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFD6E3BC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -388,11 +478,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -457,6 +544,9 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,6 +557,38 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,7 +650,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -580,7 +702,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -774,24 +896,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1FF0E3-B986-4CBD-A954-50305D7509CF}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.36328125" customWidth="1"/>
-    <col min="2" max="2" width="44.36328125" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="53.90625" customWidth="1"/>
     <col min="4" max="4" width="36.54296875" customWidth="1"/>
     <col min="5" max="5" width="39.90625" customWidth="1"/>
@@ -806,19 +928,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
-      <c r="C1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>44571</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11"/>
+      <c r="G1" s="10"/>
       <c r="H1" s="28" t="s">
         <v>3</v>
       </c>
@@ -829,117 +951,214 @@
         <v>4</v>
       </c>
       <c r="B2" s="26"/>
-      <c r="C2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="19" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30"/>
       <c r="B3" s="26"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="16" t="s">
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="H4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B5" s="26"/>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="G6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="I6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35"/>
+    </row>
+    <row r="7" spans="1:9" s="33" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:9" s="38" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="38" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="38" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="42" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+    </row>
+    <row r="18" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="H1:I1"/>
@@ -949,5 +1168,6 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Test cases for Address and My Profile section
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="325"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Profile_Page_TestCases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
   <si>
     <t>Product Name</t>
   </si>
@@ -149,9 +149,6 @@
     <t>TC_SP_004</t>
   </si>
   <si>
-    <t>Check that user able to update profile details like Profile photo , Name .</t>
-  </si>
-  <si>
     <t>Check that after click on the profile photo user able to see the details (*Name, *Student ID, *View Profile button,  *LeaderBoard, *Students Analytics, Bookmarks, Announcement, *Conceptual sessions, *Logout button ) or not.</t>
   </si>
   <si>
@@ -194,14 +191,161 @@
     <t>TC_SP_011</t>
   </si>
   <si>
-    <t xml:space="preserve"> Test Cases For 'Profile View Section'</t>
+    <t>Check that all the buttons (My Profile, Address, Education, Job profile, Job Experience, Skill Set, Important Links, Job application, Got hired, Course Request, Order History, Certification) are navigate to right link or not</t>
+  </si>
+  <si>
+    <t>TC_SP_012</t>
+  </si>
+  <si>
+    <t>Check the status bar functionality is working properly or not</t>
+  </si>
+  <si>
+    <t>TC_SP_013</t>
+  </si>
+  <si>
+    <t>TC_SP_014</t>
+  </si>
+  <si>
+    <t>Check the Device Activity  is showing proper information or not</t>
+  </si>
+  <si>
+    <t>Check the Device Activity functionality like add device and remove device is working properly or not</t>
+  </si>
+  <si>
+    <t>TC_SP_015</t>
+  </si>
+  <si>
+    <t>Check under 'My Profile' all the information is showing with right information (*Student Id, *Full Name, *Email address, *Phone number) or not</t>
+  </si>
+  <si>
+    <t>TC_SP_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that user able to update profile details like Profile photo , Name , Password . </t>
+  </si>
+  <si>
+    <t>TC_SP_017</t>
+  </si>
+  <si>
+    <t>TC_SP_018</t>
+  </si>
+  <si>
+    <t>To verify that Name field should not accept any special characters (@, #, $, %, &amp;, *, ^, !, ~ etc) and Numbers (0, 1, 2….).</t>
+  </si>
+  <si>
+    <t>TC_SP_019</t>
+  </si>
+  <si>
+    <t>To verify that user should not change the registered Email address.</t>
+  </si>
+  <si>
+    <t>TC_SP_020</t>
+  </si>
+  <si>
+    <t>To verify that 'Upload Photo' should only accept image format files (.jpg, .png, .jpeg etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that Phone Number field should not accept character (@, A, a…. ect) and should only accept 11 digits of verified BD number. </t>
+  </si>
+  <si>
+    <t>TC_SP_021</t>
+  </si>
+  <si>
+    <t>Check that user should get verification code to detect valid number while change the mobile number.</t>
+  </si>
+  <si>
+    <t>TC_SP_022</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/bz4n7HsCPFocC8fb0iTF</t>
+  </si>
+  <si>
+    <t>TC_SP_023</t>
+  </si>
+  <si>
+    <t>Check that New Password must be 6 to 15 characters which contain at least one numeric digit and a special character! Again New Password and Retype password should be match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that to update password user should be provide valid current password </t>
+  </si>
+  <si>
+    <t>TC_SP_024</t>
+  </si>
+  <si>
+    <t>Check that while updating profile user should be give valid Name and space should not be acceptable</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/pI5PiZQBrfCebGs7LAbl</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_SP_025</t>
+  </si>
+  <si>
+    <t>To verify proper error messege display or not</t>
+  </si>
+  <si>
+    <t>TC_SP_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Cases For 'View profile (My Profile) Section'</t>
+  </si>
+  <si>
+    <t>Test Cases For 'View profile (Address) Section'</t>
+  </si>
+  <si>
+    <t>Check that Present and Parmanent addresses are properly display or not</t>
+  </si>
+  <si>
+    <t>TC_SP_028</t>
+  </si>
+  <si>
+    <t>Check that Edit button to update address is clickable or not</t>
+  </si>
+  <si>
+    <t>TC_SP_029</t>
+  </si>
+  <si>
+    <t>Check that 'Select your Country' , 'Select District' and 'Street Address' are automatically filled by registerd information or not</t>
+  </si>
+  <si>
+    <t>TC_SP_030</t>
+  </si>
+  <si>
+    <t>Check that 'Street Address' field receive only spaces or not</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/77X7UEzBQcQRo1Whim8y</t>
+  </si>
+  <si>
+    <t>TC_SP_031</t>
+  </si>
+  <si>
+    <t>Check that 'Street Address' is according to the 'Country' or not</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/u1VAlDcSVR5t9WdO1iGN</t>
+  </si>
+  <si>
+    <t>TC_SP_032</t>
+  </si>
+  <si>
+    <t>Check that display error messege when 'Street Address' input field keep blank.</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/LdQGEoGaWHCakUJocavE</t>
+  </si>
+  <si>
+    <t>Test Cases For 'View profile (Education) Section'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +412,37 @@
       <i/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -348,7 +523,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,10 +650,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -544,6 +720,26 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -558,40 +754,49 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -896,7 +1101,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -904,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,14 +1125,14 @@
     <col min="6" max="6" width="34.26953125" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" customWidth="1"/>
     <col min="8" max="8" width="17.90625" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="19" t="s">
         <v>28</v>
       </c>
@@ -941,16 +1146,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="4" t="s">
         <v>29</v>
       </c>
@@ -968,8 +1173,8 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -989,10 +1194,10 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1014,17 +1219,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>18</v>
       </c>
@@ -1059,105 +1264,311 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="33" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:9" s="27" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-    </row>
-    <row r="8" spans="1:9" s="38" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" s="32" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="38" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:9" s="32" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="38" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:9" s="32" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="32" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="B11" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="32" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B12" s="40" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
+    <row r="13" spans="1:9" s="32" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B13" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="39" t="s">
+    <row r="14" spans="1:9" s="32" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B14" s="40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
+    <row r="15" spans="1:9" s="32" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B15" s="40" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
+    <row r="16" spans="1:9" s="32" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B16" s="40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+    </row>
+    <row r="18" spans="1:9" s="32" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="39" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="42" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="41" t="s">
+      <c r="B18" s="40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="32" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-    </row>
-    <row r="18" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>40</v>
-      </c>
+      <c r="B19" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="32" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="32" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="32" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="32" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="32" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="32" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="32" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="32" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="32" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="32" customFormat="1" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="32" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="32" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" s="52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="32" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="43" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+    </row>
+    <row r="36" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="43" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
@@ -1167,7 +1578,14 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I26" r:id="rId1"/>
+    <hyperlink ref="I31" r:id="rId2"/>
+    <hyperlink ref="I39" r:id="rId3"/>
+    <hyperlink ref="I40" r:id="rId4"/>
+    <hyperlink ref="I41" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Test Cases for MyClasses section
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="180">
   <si>
     <t>Product Name</t>
   </si>
@@ -284,9 +284,6 @@
     <t>TC_SP_025</t>
   </si>
   <si>
-    <t>To verify proper error messege display or not</t>
-  </si>
-  <si>
     <t>TC_SP_027</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>TC_SP_032</t>
   </si>
   <si>
-    <t>Check that display error messege when 'Street Address' input field keep blank.</t>
-  </si>
-  <si>
     <t>https://watch.screencastify.com/v/LdQGEoGaWHCakUJocavE</t>
   </si>
   <si>
@@ -374,9 +368,6 @@
     <t>TC_SP_037</t>
   </si>
   <si>
-    <t>Check that in the 'Important Link' section when user want to give only spaces or invalid input then it should be display error messeges.</t>
-  </si>
-  <si>
     <t>TC_SP_038</t>
   </si>
   <si>
@@ -416,9 +407,6 @@
     <t>TC_SP_043</t>
   </si>
   <si>
-    <t>Check that after upload a profile photo click to the other link without save then warning messege show or not</t>
-  </si>
-  <si>
     <t>https://watch.screencastify.com/v/CHzXFPOH46wp6RO3RPge</t>
   </si>
   <si>
@@ -453,6 +441,132 @@
   </si>
   <si>
     <t>Check that after click on 'Continue Course' button it's navigate to the proper page or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_049</t>
+  </si>
+  <si>
+    <t>Check that after click on 'Continue Course' button videos should not play automatically without users permission.</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/a0gq0wlI2gGUA76M3HtM</t>
+  </si>
+  <si>
+    <t>TC_SP_050</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to scroll videos or not.</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to click on the video or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_052</t>
+  </si>
+  <si>
+    <t>TC_SP_051</t>
+  </si>
+  <si>
+    <t>Verify that the user can pause the video or not</t>
+  </si>
+  <si>
+    <t>TC_SP_053</t>
+  </si>
+  <si>
+    <t>Verify that the user can mute the video or not</t>
+  </si>
+  <si>
+    <t>TC_SP_054</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to increase and decrease the volume or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_055</t>
+  </si>
+  <si>
+    <t>TC_SP_056</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to select video quality from the list.</t>
+  </si>
+  <si>
+    <t>TC_SP_057</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to select video speed from the list.</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to change the screen size or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_058</t>
+  </si>
+  <si>
+    <t>To verify proper error message display or not</t>
+  </si>
+  <si>
+    <t>Check that display error message when 'Street Address' input field keep blank.</t>
+  </si>
+  <si>
+    <t>Check that in the 'Important Link' section when user want to give only spaces or invalid input then it should be display error messages.</t>
+  </si>
+  <si>
+    <t>Check that after upload a profile photo click to the other link without save then warning message show or not</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/HQahJ4CSWi50v9kZ8ZDK</t>
+  </si>
+  <si>
+    <t>TC_SP_059</t>
+  </si>
+  <si>
+    <t>Verify that at the video playing time if the internet connection will suddenly disconnected and if restored the connection then error message should not be displayed continue.</t>
+  </si>
+  <si>
+    <t>Verify that 'Previous' and 'Next' button is working properly or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_060</t>
+  </si>
+  <si>
+    <t>Verify that 'Bookmark' link is properly working or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_061</t>
+  </si>
+  <si>
+    <t>Verify that 'Course Content' progress bar is working properly.</t>
+  </si>
+  <si>
+    <t>TC_SP_062</t>
+  </si>
+  <si>
+    <t>Verify that 'Copyright warning' link shows the right message or nor.</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/PbI7mhfPah9TiixmaXMR</t>
+  </si>
+  <si>
+    <t>TC_SP_063</t>
+  </si>
+  <si>
+    <t>To verify that the search result is displayed as per the search query.</t>
+  </si>
+  <si>
+    <t>TC_SP_064</t>
+  </si>
+  <si>
+    <t>To verify that the user is able to do a blank search or not</t>
+  </si>
+  <si>
+    <t>TC_SP_065</t>
+  </si>
+  <si>
+    <t>To verify that 'Complete Course' button navigate the proper page or not.</t>
   </si>
 </sst>
 </file>
@@ -562,7 +676,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +752,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,7 +888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -891,22 +1011,25 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1215,7 +1338,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1223,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1243,7 +1366,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="48"/>
@@ -1260,13 +1383,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="10"/>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="50"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="49" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="48"/>
@@ -1287,7 +1410,7 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="48"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
@@ -1308,7 +1431,7 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="49" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="48"/>
@@ -1333,17 +1456,17 @@
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="51" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="48"/>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="17" t="s">
         <v>18</v>
       </c>
@@ -1461,11 +1584,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
+      <c r="A17" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
@@ -1596,252 +1719,406 @@
         <v>84</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>85</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A35" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B35" s="45"/>
       <c r="C35" s="45"/>
     </row>
     <row r="36" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="38" t="s">
         <v>90</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="40" t="s">
         <v>92</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="38" t="s">
         <v>94</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>95</v>
       </c>
       <c r="G39" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I39" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="38" t="s">
         <v>97</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>98</v>
       </c>
       <c r="G40" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="G41" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I41" s="35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A44" s="45" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B44" s="45"/>
       <c r="C44" s="45"/>
     </row>
     <row r="45" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G45" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B46" s="41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" s="41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G47" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B48" s="41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G48" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I48" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B49" s="41" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B50" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B52" s="41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G54" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I54" s="35" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="39" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B55" s="41" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="G55" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I55" s="35" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B56" s="41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A59" s="45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B59" s="45"/>
       <c r="C59" s="45"/>
     </row>
     <row r="60" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B60" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="39" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B62" s="41" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I64" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="B63" s="41" t="s">
+    </row>
+    <row r="65" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="39" t="s">
         <v>141</v>
+      </c>
+      <c r="B65" s="41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="41" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" s="41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71" s="41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" s="41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G73" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I73" s="35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B74" s="41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" s="41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B77" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="G77" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="I77" s="35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" s="41" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="41" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1869,8 +2146,11 @@
     <hyperlink ref="I48" r:id="rId8"/>
     <hyperlink ref="I54" r:id="rId9"/>
     <hyperlink ref="I55" r:id="rId10"/>
+    <hyperlink ref="I64" r:id="rId11"/>
+    <hyperlink ref="I73" r:id="rId12"/>
+    <hyperlink ref="I77" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
start execution the TestCases and finding bugs
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="367">
   <si>
     <t>Product Name</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>REMARKS</t>
   </si>
   <si>
     <t>COMMENTS</t>
@@ -125,9 +122,6 @@
     <t>Windows, Android</t>
   </si>
   <si>
-    <t>Verify that system redirecting user to valid page or not when user click on 'Login' Button from Welcome page.</t>
-  </si>
-  <si>
     <t>TC_SP_001</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>TC_SP_003</t>
   </si>
   <si>
-    <t>Check that  *Profile name , *Profile Photo and other important links like *My Classes, Support, *Notification Icon, Shopping Icon, Diamond icon, Programming Hero Logo  are  Showing or not.</t>
-  </si>
-  <si>
     <t>TC_SP_004</t>
   </si>
   <si>
@@ -230,9 +221,6 @@
     <t>TC_SP_018</t>
   </si>
   <si>
-    <t>To verify that Name field should not accept any special characters (@, #, $, %, &amp;, *, ^, !, ~ etc) and Numbers (0, 1, 2….).</t>
-  </si>
-  <si>
     <t>TC_SP_019</t>
   </si>
   <si>
@@ -272,12 +260,6 @@
     <t>TC_SP_024</t>
   </si>
   <si>
-    <t>Check that while updating profile user should be give valid Name and space should not be acceptable</t>
-  </si>
-  <si>
-    <t>https://watch.screencastify.com/v/pI5PiZQBrfCebGs7LAbl</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -344,18 +326,12 @@
     <t>TC_SP_035</t>
   </si>
   <si>
-    <t xml:space="preserve">Check that system should not accept only spaces for 'Job Title', 'Company Name' and 'Description' input field </t>
-  </si>
-  <si>
     <t>https://watch.screencastify.com/v/pzbC2SWEeHg9ENuobpFp</t>
   </si>
   <si>
     <t>TC_SP_036</t>
   </si>
   <si>
-    <t xml:space="preserve">Check that in the 'Skill Set' section to 'Take a skill test' skill test questions should be available and display. </t>
-  </si>
-  <si>
     <t>https://watch.screencastify.com/v/VtverlxHbhbw8R4Me6oK</t>
   </si>
   <si>
@@ -371,9 +347,6 @@
     <t>TC_SP_039</t>
   </si>
   <si>
-    <t>Check that in the 'Order Hostory' section proper imformation is display or not.</t>
-  </si>
-  <si>
     <t>TC_SP_040</t>
   </si>
   <si>
@@ -509,9 +482,6 @@
     <t>TC_SP_059</t>
   </si>
   <si>
-    <t>Verify that at the video playing time if the internet connection will suddenly disconnected and if restored the connection then error message should not be displayed continue.</t>
-  </si>
-  <si>
     <t>Verify that 'Previous' and 'Next' button is working properly or not.</t>
   </si>
   <si>
@@ -684,13 +654,589 @@
   </si>
   <si>
     <t>Check that 'Announcement' button navigate the user to the proper link page and display the right information.</t>
+  </si>
+  <si>
+    <t>Verify that the system redirecting user to valid page or not when user input valid email and password and click on 'Login' Button from Welcome page.</t>
+  </si>
+  <si>
+    <t>Test Cases for 'Logout' button</t>
+  </si>
+  <si>
+    <t>TC_SP_083</t>
+  </si>
+  <si>
+    <t>TC_SP_084</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Click on profile icon to check 'Logout' button is visible or not.</t>
+  </si>
+  <si>
+    <t>Verify  by Click on 'Logout' button without internet Connection and reconnect to internet check it’s properly logout or not.</t>
+  </si>
+  <si>
+    <t>TC_SP_085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not click on 'Logout' button and close the browser,
+reopen the application by hitting the URL and application
+should not be logged out.
+</t>
+  </si>
+  <si>
+    <t>TC_SP_086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on Log out button and now press the back button of
+browser. It should not show the user logged into the
+application, user should be on log in screen.
+</t>
+  </si>
+  <si>
+    <t>TC_SP_087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open browser and hit the application with URL, open a new
+tab within the same browser, now click on log out from one
+tab and user should be logged out after clicking on any
+operation from the application.
+</t>
+  </si>
+  <si>
+    <t>TC_SP_088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the logout button and user should be logged out
+from the application
+</t>
+  </si>
+  <si>
+    <t>Test Cases for 'UI' Part</t>
+  </si>
+  <si>
+    <t>TC_SP_089</t>
+  </si>
+  <si>
+    <t>Check that the website is responsive for other devices (Mobile, Tab etc) and all browsers (Google chrome, Mozilla firefox etc)</t>
+  </si>
+  <si>
+    <t>TC_SP_090</t>
+  </si>
+  <si>
+    <t>Check that 'Search Box' is available on the header section to search the full website contents.</t>
+  </si>
+  <si>
+    <t>TC_SP_091</t>
+  </si>
+  <si>
+    <t>Check that all placeholders for input fields are displayed or not</t>
+  </si>
+  <si>
+    <t>TC_SP_092</t>
+  </si>
+  <si>
+    <t>Check that keyboard keys (Tab, Enter, Space bar etc) are working perfectly or not.</t>
+  </si>
+  <si>
+    <t>1. open browser
+2. visit https://web.programming-hero.com/
+3. click on 'Login' button from navigation menu
+4. type valid email and password
+5. click on 'Login' button (ER-1)</t>
+  </si>
+  <si>
+    <t>registered email and password
+(not given here for security reason)</t>
+  </si>
+  <si>
+    <t>1. User should successfully Login and display the dashboard.</t>
+  </si>
+  <si>
+    <t>Displayed dashboard successfully.</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>1. All the expected field should be displayed.</t>
+  </si>
+  <si>
+    <t>Check that  *User name , *Profile Photo and other important links like *My Classes, Support, *Notification Icon, Shopping Icon, Diamond icon, Programming Hero Logo  are  Showing or not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profile Photo and other important links are showing but the registered user name is not displaying under the phofile photo.  </t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>All the expected field should be displayed.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Student ID is not displaying</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Bookmark' button</t>
+  </si>
+  <si>
+    <t>User should navigate to the proper page</t>
+  </si>
+  <si>
+    <t>Proper page is displaying</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Student Analytics' button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Leader Board' button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Announcement' button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Conceptual Session' button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'Logout' button</t>
+  </si>
+  <si>
+    <t>User should be Logged out</t>
+  </si>
+  <si>
+    <t>User Logging out successfully</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button</t>
+  </si>
+  <si>
+    <t>Status Bar should display with proper percentage</t>
+  </si>
+  <si>
+    <t>Should be display the list of active device name, date and time</t>
+  </si>
+  <si>
+    <t>Not displaying properly everytime</t>
+  </si>
+  <si>
+    <t>Should be remove from the list</t>
+  </si>
+  <si>
+    <t>removed successfully</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Remove' button</t>
+  </si>
+  <si>
+    <t>Should be display all the information perfectly</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button</t>
+  </si>
+  <si>
+    <t>All field should be editable.</t>
+  </si>
+  <si>
+    <t>Update is working.</t>
+  </si>
+  <si>
+    <t>Email Address cannot be changed</t>
+  </si>
+  <si>
+    <t>Email field is disabled</t>
+  </si>
+  <si>
+    <t>Name : R&amp;*@</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/xfPJdJEQH3a946xr6h1T</t>
+  </si>
+  <si>
+    <t>To verify that Name field should not accept any special characters (@, #, $, %, &amp;, *, ^, !, ~ etc), only spaces and Numbers (0, 1, 2….).</t>
+  </si>
+  <si>
+    <t>Should not accept special characters, only spaces and numbers.</t>
+  </si>
+  <si>
+    <t>Name field accepts wrong inputs.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button
+4. input data to 'Name' field</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button
+4. input data to 'Phone' field</t>
+  </si>
+  <si>
+    <t>Phone: 1234</t>
+  </si>
+  <si>
+    <t>Should not accept less than or greater than 11 digits</t>
+  </si>
+  <si>
+    <t>Phone field accepts wrong mobile number.</t>
+  </si>
+  <si>
+    <t>input a valid mobile number
+(01682706635)</t>
+  </si>
+  <si>
+    <t>User need to get a validation code</t>
+  </si>
+  <si>
+    <t>No validation code have received</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button
+4. upload an image file</t>
+  </si>
+  <si>
+    <t>input an image file format
+ (.jpg or .png or .jpeg)</t>
+  </si>
+  <si>
+    <t>valid image file should be uploaded</t>
+  </si>
+  <si>
+    <t>accept the condition perfectly</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button
+4. input valid current password</t>
+  </si>
+  <si>
+    <t>valid current password
+(not write here for the security reason)</t>
+  </si>
+  <si>
+    <t>Check that while updating password user should be logout automatically.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Edit Profile' button
+4. input valid current password
+5. input new Password and retype password
+6. click on 'Change Password' button</t>
+  </si>
+  <si>
+    <t>not write here for the security reason</t>
+  </si>
+  <si>
+    <t>User need to logout automatically</t>
+  </si>
+  <si>
+    <t>User staying on the current page</t>
+  </si>
+  <si>
+    <t>https://watch.screencastify.com/v/wDJ9x8wK434MARg3hnQS</t>
+  </si>
+  <si>
+    <t>Proper error message should be displayed when wrong input provide.</t>
+  </si>
+  <si>
+    <t>Proper error message is displayed</t>
+  </si>
+  <si>
+    <t>give some invalid input</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Address' button</t>
+  </si>
+  <si>
+    <t>Proper address should be displayed</t>
+  </si>
+  <si>
+    <t>Proper address is displayed</t>
+  </si>
+  <si>
+    <t>Address button should be clickable.</t>
+  </si>
+  <si>
+    <t>Address button is clickable</t>
+  </si>
+  <si>
+    <t>Registered information should be displayed automatically</t>
+  </si>
+  <si>
+    <t>Registered information is displayed automatically</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Address' button
+4. Click on 'Edit' Button</t>
+  </si>
+  <si>
+    <t>input only spaces</t>
+  </si>
+  <si>
+    <t>Only spaces should not be accepted.</t>
+  </si>
+  <si>
+    <t>Only spaces is accepted.</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Address' button
+4. Click on 'Edit' Button
+5. input data to the 'Street Address' field</t>
+  </si>
+  <si>
+    <t>input any place name which is not according to the Country name.</t>
+  </si>
+  <si>
+    <t>Input data should be check first, then update</t>
+  </si>
+  <si>
+    <t>Accept place name which is not belongs to the Country name.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Address' button
+4. Click on 'Edit' Button
+5. input no data to the 'Street Address' field</t>
+  </si>
+  <si>
+    <t>Should be displayed error message.</t>
+  </si>
+  <si>
+    <t>No error message is displayed.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Education' button
+4. Click on 'Edit' Button
+5. input data</t>
+  </si>
+  <si>
+    <t>Exam Name/Title : 123
+Institution Name: 12345</t>
+  </si>
+  <si>
+    <t>Should not accept invalid data.</t>
+  </si>
+  <si>
+    <t>Already accepted invalid data.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Education' button
+4. Click on 'Edit' Button
+5. input only spaces</t>
+  </si>
+  <si>
+    <t>Should be displayed error message</t>
+  </si>
+  <si>
+    <t>Correct error message is displayed.</t>
+  </si>
+  <si>
+    <t>Check that system should not accept only spaces for 'Job Title', 'Company Name' and 'Description' input field for the 'Job Experience' section</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Job Experience' button
+4. Click on 'Add Experience' Button
+5. input only spaces</t>
+  </si>
+  <si>
+    <t>Should not accept only spaces as data.</t>
+  </si>
+  <si>
+    <t>Already accepted only spaces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that in the 'Skill Set' section, to 'Take a skill test' skill test questions should be available and display. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Skill Set' button
+4. Click on 'Take a skill Test' Button
+</t>
+  </si>
+  <si>
+    <t>Some Questions should be displayed to take skill test.</t>
+  </si>
+  <si>
+    <t>Not available</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Important Links' button</t>
+  </si>
+  <si>
+    <t>Error message should be displayed</t>
+  </si>
+  <si>
+    <t>Error message is displayed properly</t>
+  </si>
+  <si>
+    <t>Check that in the 'Order History' section proper imformation is display or not.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Order History' button</t>
+  </si>
+  <si>
+    <t>All the information should be displayed properly</t>
+  </si>
+  <si>
+    <t>Information is displayed correctly.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'Order History' button
+4. Click on 'Invoice Download' button</t>
+  </si>
+  <si>
+    <t>Invoice should be downloaded.</t>
+  </si>
+  <si>
+    <t>Proper invoice is download successfully</t>
+  </si>
+  <si>
+    <t>New updated profile photo should be displayed.</t>
+  </si>
+  <si>
+    <t>Updated photo is displayed.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'My Profile' button
+4. Click on 'Upload Photo' button</t>
+  </si>
+  <si>
+    <t>upload a right format image</t>
+  </si>
+  <si>
+    <t>User should be able to crop the image.</t>
+  </si>
+  <si>
+    <t>Not cropable</t>
+  </si>
+  <si>
+    <t>Alert message should be displayed.</t>
+  </si>
+  <si>
+    <t>No alert message is displayed</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'My Profile' button
+4. Click on 'Upload Photo' button
+5. Click on another link or button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on 'View Profile' button
+3. Click on 'My Profile' button
+4. Click on 'Upload Photo' button
+5. Select multiple photo to upload</t>
+  </si>
+  <si>
+    <t>Should not possible</t>
+  </si>
+  <si>
+    <t>not possible to upload multiple photo at a time</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Classes'</t>
+  </si>
+  <si>
+    <t>User should be navigate to the right page.</t>
+  </si>
+  <si>
+    <t>Navigate to the right page.</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on  'ক্লিক করুন' button</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Click on  'ক্লিক করুন' button
+3. Click on the FB link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'My Classes'
+2. Click on  'Continue' button
+</t>
+  </si>
+  <si>
+    <t>Video should not play without user's permission</t>
+  </si>
+  <si>
+    <t>Video is playing automatically</t>
+  </si>
+  <si>
+    <t>1. Click on 'My Classes'
+2. Click on  'Continue' button</t>
+  </si>
+  <si>
+    <t>Playlist should be scrollable</t>
+  </si>
+  <si>
+    <t>scrollable perfectly</t>
+  </si>
+  <si>
+    <t>Verify that, at the video playing time if the internet connection will suddenly disconnected and if restored the connection then error message should not be displayed continue.</t>
+  </si>
+  <si>
+    <t>Video should be continue without any interrupt.</t>
+  </si>
+  <si>
+    <t>Video is interrupted with showing error message which is really disturbing.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,8 +1346,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,18 +1446,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor rgb="FFD6E3BC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -892,8 +1462,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD6E3BC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1014,12 +1602,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1085,19 +1686,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1111,26 +1699,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1139,12 +1709,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1155,19 +1726,64 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1185,6 +1801,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>74083</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>96836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1181101</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>927100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="17758833" y="15743236"/>
+          <a:ext cx="1107018" cy="830264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1476,7 +2141,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1484,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1503,13 +2168,13 @@
     <col min="9" max="9" width="34.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:10" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1520,24 +2185,28 @@
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="47" t="s">
+      <c r="G1" s="10">
+        <v>44572</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="47"/>
-    </row>
-    <row r="2" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="I1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="49"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>44572</v>
+      </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1547,9 +2216,9 @@
       </c>
       <c r="I2" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="50"/>
-      <c r="B3" s="49"/>
+    <row r="3" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="40"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -1561,20 +2230,20 @@
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="49"/>
+    <row r="4" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="39"/>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>12</v>
@@ -1593,24 +2262,24 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="52" t="s">
+    <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="52" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" s="55" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" s="36" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>19</v>
       </c>
@@ -1633,815 +2302,2242 @@
         <v>25</v>
       </c>
       <c r="H6" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="27" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="26" t="s">
+    </row>
+    <row r="7" spans="1:10" s="53" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="54"/>
+    </row>
+    <row r="8" spans="1:10" s="27" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:9" s="32" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+      <c r="B8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="C8" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="44"/>
+    </row>
+    <row r="9" spans="1:10" s="27" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:10" s="27" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="32" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C10" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" s="44"/>
+    </row>
+    <row r="11" spans="1:10" s="27" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="32" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="30" t="s">
+      <c r="B11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G11" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="44"/>
+    </row>
+    <row r="12" spans="1:10" s="27" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B12" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="44"/>
+    </row>
+    <row r="13" spans="1:10" s="27" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="I10" s="44" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="32" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="s">
+      <c r="B13" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" s="27" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B14" s="29" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="32" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
+      <c r="C14" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G14" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="44"/>
+    </row>
+    <row r="15" spans="1:10" s="27" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B15" s="29" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="32" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="33" t="s">
+      <c r="C15" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="44"/>
+    </row>
+    <row r="16" spans="1:10" s="27" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>255</v>
+      </c>
+      <c r="G16" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="44"/>
+    </row>
+    <row r="17" spans="1:10" s="31" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="45"/>
+    </row>
+    <row r="18" spans="1:10" s="27" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="32" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="34" t="s">
+      <c r="B18" s="29" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="32" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="34" t="s">
+      <c r="C18" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>247</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="G18" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="44"/>
+    </row>
+    <row r="19" spans="1:10" s="27" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="32" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-    </row>
-    <row r="18" spans="1:9" s="32" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
+      <c r="B19" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="C19" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="44"/>
+    </row>
+    <row r="20" spans="1:10" s="27" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="32" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="B20" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="44"/>
+    </row>
+    <row r="21" spans="1:10" s="27" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="32" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
+      <c r="B21" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="C21" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="G21" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="44"/>
+    </row>
+    <row r="22" spans="1:10" s="27" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="32" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="34" t="s">
+      <c r="C22" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="H22" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="J22" s="44"/>
+    </row>
+    <row r="23" spans="1:10" s="27" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="32" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="33" t="s">
+      <c r="B23" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="C23" s="49" t="s">
+        <v>264</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>266</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="44"/>
+    </row>
+    <row r="24" spans="1:10" s="27" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="32" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="33" t="s">
+      <c r="B24" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="44"/>
+    </row>
+    <row r="25" spans="1:10" s="27" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B25" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="E25" s="62" t="s">
+        <v>272</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I25" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="J25" s="44"/>
+    </row>
+    <row r="26" spans="1:10" s="27" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" s="32" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="34" t="s">
+      <c r="B26" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I26" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="44"/>
+    </row>
+    <row r="27" spans="1:10" s="27" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>279</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>280</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="J27" s="44"/>
+    </row>
+    <row r="28" spans="1:10" s="27" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" s="32" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="34" t="s">
+      <c r="B28" s="29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" s="32" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="I26" s="44" t="s">
+      <c r="C28" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>283</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="F28" s="48" t="s">
+        <v>285</v>
+      </c>
+      <c r="G28" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="44"/>
+    </row>
+    <row r="29" spans="1:10" s="27" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="44"/>
+    </row>
+    <row r="30" spans="1:10" s="27" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="44"/>
+    </row>
+    <row r="31" spans="1:10" s="27" customFormat="1" ht="107.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" s="32" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="32" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="32" customFormat="1" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="32" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="33" t="s">
+      <c r="B31" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="F31" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="G31" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="H31" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="J31" s="44"/>
+    </row>
+    <row r="32" spans="1:10" s="27" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" s="32" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="G31" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="I31" s="44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="32" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="G32" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="44"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A35" s="46" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B35" s="46"/>
       <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="F36" s="48" t="s">
+        <v>299</v>
+      </c>
+      <c r="G36" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+    </row>
+    <row r="37" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B39" s="48" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="39" t="s">
+      <c r="C39" s="49" t="s">
+        <v>304</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E39" s="48" t="s">
+        <v>306</v>
+      </c>
+      <c r="F39" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="27"/>
+      <c r="I39" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="38" t="s">
+    </row>
+    <row r="40" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="25" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="39" t="s">
+      <c r="B40" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="C40" s="49" t="s">
+        <v>309</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="E40" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="G40" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="H40" s="61" t="s">
+        <v>308</v>
+      </c>
+      <c r="I40" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="39" t="s">
+    <row r="41" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B41" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E41" s="48" t="s">
+        <v>314</v>
+      </c>
+      <c r="F41" s="48" t="s">
+        <v>315</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I41" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="G39" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I39" s="35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I40" s="35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>155</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I41" s="35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+    </row>
+    <row r="44" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A44" s="46" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B44" s="46"/>
       <c r="C44" s="46"/>
-    </row>
-    <row r="45" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="39" t="s">
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+    </row>
+    <row r="45" spans="1:9" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="D45" s="62" t="s">
+        <v>317</v>
+      </c>
+      <c r="E45" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="F45" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H45" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I45" s="33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="D46" s="48" t="s">
+        <v>305</v>
+      </c>
+      <c r="E46" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="F46" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="G46" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E47" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="F47" s="48" t="s">
+        <v>326</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I47" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="41" t="s">
+    </row>
+    <row r="48" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="G45" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I45" s="35" t="s">
+      <c r="B48" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>328</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I48" s="33" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="39" t="s">
+    <row r="49" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B49" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>331</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E49" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="F49" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="G49" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="27"/>
+      <c r="I49" s="27"/>
+    </row>
+    <row r="50" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="39" t="s">
+      <c r="B50" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="C50" s="27"/>
+      <c r="D50" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+    </row>
+    <row r="51" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="G47" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I47" s="35" t="s">
+      <c r="B51" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="F51" s="48" t="s">
+        <v>337</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+    </row>
+    <row r="52" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="39" t="s">
+      <c r="B52" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="C52" s="49" t="s">
+        <v>338</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E52" s="48" t="s">
+        <v>339</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="G52" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="G48" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I48" s="35" t="s">
+      <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="39" t="s">
+      <c r="C53" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="F53" s="48" t="s">
+        <v>342</v>
+      </c>
+      <c r="G53" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+    </row>
+    <row r="54" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="41" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="39" t="s">
+      <c r="B54" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="C54" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="E54" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="F54" s="48" t="s">
+        <v>346</v>
+      </c>
+      <c r="G54" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I54" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="39" t="s">
+    <row r="55" spans="1:9" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="41" t="s">
+      <c r="B55" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>344</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>347</v>
+      </c>
+      <c r="F55" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="61" t="s">
+        <v>240</v>
+      </c>
+      <c r="I55" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="39" t="s">
+    <row r="56" spans="1:9" ht="99.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B56" s="26" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B54" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="G54" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I54" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="B55" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="G55" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I55" s="35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B56" s="41" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C56" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="D56" s="27"/>
+      <c r="E56" s="48" t="s">
+        <v>351</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="G56" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="27"/>
+    </row>
+    <row r="59" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A59" s="46" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B59" s="46"/>
       <c r="C59" s="46"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
     </row>
     <row r="60" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E60" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="F60" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="G60" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
+    </row>
+    <row r="61" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E61" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="F61" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="G61" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+    </row>
+    <row r="62" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E62" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="F62" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="G62" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="27"/>
+      <c r="I62" s="27"/>
+    </row>
+    <row r="63" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="27"/>
+      <c r="D63" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" s="48" t="s">
+        <v>354</v>
+      </c>
+      <c r="F63" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="G63" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="27"/>
+      <c r="I63" s="27"/>
+    </row>
+    <row r="64" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="C64" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="F64" s="48" t="s">
+        <v>360</v>
+      </c>
+      <c r="G64" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H64" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I64" s="33" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="39" t="s">
+    <row r="65" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B65" s="26" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="39" t="s">
+      <c r="C65" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="G65" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="27"/>
+      <c r="I65" s="27"/>
+    </row>
+    <row r="66" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="C66" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" s="27"/>
+      <c r="I66" s="27"/>
+    </row>
+    <row r="67" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="25" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="B63" s="41" t="s">
+      <c r="B67" s="26" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="39" t="s">
+      <c r="C67" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D67" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="27"/>
+      <c r="I67" s="27"/>
+    </row>
+    <row r="68" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B68" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="G64" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I64" s="35" t="s">
+      <c r="C68" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D68" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="27"/>
+      <c r="I68" s="27"/>
+    </row>
+    <row r="69" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="25" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="39" t="s">
+      <c r="B69" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="C69" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
+    </row>
+    <row r="70" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="25" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="39" t="s">
+      <c r="B70" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D70" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E70" s="27"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="27"/>
+      <c r="I70" s="27"/>
+    </row>
+    <row r="71" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" s="27"/>
+      <c r="I71" s="27"/>
+    </row>
+    <row r="72" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="B66" s="41" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="B67" s="41" t="s">
+      <c r="B72" s="26" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" s="41" t="s">
+      <c r="C72" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D72" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="27"/>
+      <c r="I72" s="27"/>
+    </row>
+    <row r="73" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="25" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B69" s="41" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="B70" s="41" t="s">
+      <c r="B73" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="E73" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="G73" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H73" s="61" t="s">
+        <v>244</v>
+      </c>
+      <c r="I73" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="27"/>
+    </row>
+    <row r="75" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="25" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="B71" s="41" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="B72" s="41" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="39" t="s">
+      <c r="B75" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="41" t="s">
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="27"/>
+    </row>
+    <row r="76" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="27"/>
+    </row>
+    <row r="77" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="H77" s="27"/>
+      <c r="I77" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="G73" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I73" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="B74" s="41" t="s">
+      <c r="B78" s="26" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="39" t="s">
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="27"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="27"/>
+      <c r="I78" s="27"/>
+    </row>
+    <row r="79" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B79" s="26" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="39" t="s">
+      <c r="C79" s="27"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="27"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="27"/>
+    </row>
+    <row r="80" spans="1:9" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B80" s="26" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="39" t="s">
+      <c r="C80" s="27"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="27"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="27"/>
+      <c r="I80" s="27"/>
+    </row>
+    <row r="81" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B81" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="G77" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="I77" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="39" t="s">
-        <v>170</v>
-      </c>
-      <c r="B78" s="41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="B79" s="41" t="s">
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="27"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="27"/>
+      <c r="H82" s="27"/>
+      <c r="I82" s="27"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="27"/>
+    </row>
+    <row r="84" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="46" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="B80" s="41" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="B81" s="41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="46" t="s">
-        <v>183</v>
       </c>
       <c r="B84" s="46"/>
       <c r="C84" s="46"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="47"/>
     </row>
     <row r="85" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="27"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="27"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="27"/>
+      <c r="I85" s="27"/>
+    </row>
+    <row r="86" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H86" s="27"/>
+      <c r="I86" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+    </row>
+    <row r="88" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H88" s="27"/>
+      <c r="I88" s="27"/>
+    </row>
+    <row r="89" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="27"/>
+      <c r="I89" s="27"/>
+    </row>
+    <row r="90" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="B85" s="41" t="s">
+      <c r="B90" s="26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="39" t="s">
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="27"/>
+      <c r="F90" s="27"/>
+      <c r="G90" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="H90" s="27"/>
+      <c r="I90" s="27"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="27"/>
+      <c r="I91" s="27"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="27"/>
+      <c r="D92" s="27"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="27"/>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+      <c r="I92" s="27"/>
+    </row>
+    <row r="93" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="46" t="s">
         <v>186</v>
-      </c>
-      <c r="B86" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="G86" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I86" s="35" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="B87" s="41" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B88" s="41" t="s">
-        <v>192</v>
-      </c>
-      <c r="G88" s="36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="B89" s="41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B90" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="G90" s="56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="46" t="s">
-        <v>196</v>
       </c>
       <c r="B93" s="46"/>
       <c r="C93" s="46"/>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="47"/>
+      <c r="H93" s="47"/>
+      <c r="I93" s="47"/>
     </row>
     <row r="94" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="39" t="s">
+      <c r="A94" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="27"/>
+      <c r="H94" s="27"/>
+      <c r="I94" s="27"/>
+    </row>
+    <row r="95" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B95" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="27"/>
+      <c r="I95" s="27"/>
+    </row>
+    <row r="96" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="27"/>
+      <c r="I96" s="27"/>
+    </row>
+    <row r="97" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="27"/>
+      <c r="I97" s="27"/>
+    </row>
+    <row r="98" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="B94" s="41" t="s">
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H98" s="27"/>
+      <c r="I98" s="33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="27"/>
+      <c r="H99" s="27"/>
+      <c r="I99" s="27"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="27"/>
+      <c r="I100" s="27"/>
+    </row>
+    <row r="101" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="46" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="B95" s="41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="39" t="s">
-        <v>201</v>
-      </c>
-      <c r="B96" s="41" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="B97" s="41" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B98" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="G98" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="I98" s="35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" s="37" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="46" t="s">
-        <v>208</v>
       </c>
       <c r="B101" s="46"/>
       <c r="C101" s="46"/>
+      <c r="D101" s="47"/>
+      <c r="E101" s="47"/>
+      <c r="F101" s="47"/>
+      <c r="G101" s="47"/>
+      <c r="H101" s="47"/>
+      <c r="I101" s="47"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
+      <c r="G102" s="27"/>
+      <c r="H102" s="27"/>
+      <c r="I102" s="27"/>
     </row>
     <row r="103" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="B103" s="41" t="s">
+      <c r="A103" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="B103" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="27"/>
+      <c r="H103" s="27"/>
+      <c r="I103" s="27"/>
+    </row>
+    <row r="104" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="H104" s="27"/>
+      <c r="I104" s="27"/>
+    </row>
+    <row r="105" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="27"/>
+      <c r="G105" s="27"/>
+      <c r="H105" s="27"/>
+      <c r="I105" s="27"/>
+    </row>
+    <row r="106" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B106" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="27"/>
+      <c r="H106" s="27"/>
+      <c r="I106" s="27"/>
+    </row>
+    <row r="107" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="27"/>
+      <c r="I107" s="27"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="27"/>
+      <c r="G108" s="27"/>
+      <c r="H108" s="27"/>
+      <c r="I108" s="27"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="27"/>
+      <c r="I109" s="27"/>
+    </row>
+    <row r="110" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="46" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="39" t="s">
+      <c r="B110" s="46"/>
+      <c r="C110" s="46"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="47"/>
+      <c r="G110" s="47"/>
+      <c r="H110" s="47"/>
+      <c r="I110" s="47"/>
+    </row>
+    <row r="111" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="B104" s="41" t="s">
+      <c r="B111" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="27"/>
+      <c r="G111" s="27"/>
+      <c r="H111" s="27"/>
+      <c r="I111" s="27"/>
+    </row>
+    <row r="112" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="25" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="39" t="s">
-        <v>213</v>
-      </c>
-      <c r="B105" s="41" t="s">
+      <c r="B112" s="26" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="39" t="s">
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="27"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="27"/>
+      <c r="I112" s="27"/>
+    </row>
+    <row r="113" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="B113" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="27"/>
+      <c r="I113" s="27"/>
+    </row>
+    <row r="114" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="B106" s="41" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="B107" s="41" t="s">
+      <c r="B114" s="49" t="s">
         <v>218</v>
       </c>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="27"/>
+      <c r="H114" s="27"/>
+      <c r="I114" s="27"/>
+    </row>
+    <row r="115" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="27"/>
+      <c r="I115" s="27"/>
+    </row>
+    <row r="116" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="27"/>
+      <c r="G116" s="27"/>
+      <c r="H116" s="27"/>
+      <c r="I116" s="27"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="27"/>
+      <c r="G117" s="27"/>
+      <c r="H117" s="27"/>
+      <c r="I117" s="27"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
+      <c r="E118" s="27"/>
+      <c r="F118" s="27"/>
+      <c r="G118" s="27"/>
+      <c r="H118" s="27"/>
+      <c r="I118" s="27"/>
+    </row>
+    <row r="119" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="B119" s="46"/>
+      <c r="C119" s="46"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="47"/>
+      <c r="F119" s="47"/>
+      <c r="G119" s="47"/>
+      <c r="H119" s="47"/>
+      <c r="I119" s="47"/>
+    </row>
+    <row r="120" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="B120" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="C120" s="27"/>
+      <c r="D120" s="27"/>
+      <c r="E120" s="27"/>
+      <c r="F120" s="27"/>
+      <c r="G120" s="27"/>
+      <c r="H120" s="27"/>
+      <c r="I120" s="27"/>
+    </row>
+    <row r="121" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="B121" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H121" s="27"/>
+      <c r="I121" s="27"/>
+    </row>
+    <row r="122" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B122" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="C122" s="27"/>
+      <c r="D122" s="27"/>
+      <c r="E122" s="27"/>
+      <c r="F122" s="27"/>
+      <c r="G122" s="27"/>
+      <c r="H122" s="27"/>
+      <c r="I122" s="27"/>
+    </row>
+    <row r="123" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="B123" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="27"/>
+      <c r="G123" s="27"/>
+      <c r="H123" s="27"/>
+      <c r="I123" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A119:C119"/>
     <mergeCell ref="A84:C84"/>
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="A101:C101"/>
@@ -2459,23 +4555,25 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I26" r:id="rId1"/>
-    <hyperlink ref="I31" r:id="rId2"/>
-    <hyperlink ref="I39" r:id="rId3"/>
-    <hyperlink ref="I40" r:id="rId4"/>
-    <hyperlink ref="I41" r:id="rId5"/>
-    <hyperlink ref="I45" r:id="rId6"/>
-    <hyperlink ref="I47" r:id="rId7"/>
-    <hyperlink ref="I48" r:id="rId8"/>
-    <hyperlink ref="I54" r:id="rId9"/>
-    <hyperlink ref="I55" r:id="rId10"/>
-    <hyperlink ref="I64" r:id="rId11"/>
-    <hyperlink ref="I73" r:id="rId12"/>
-    <hyperlink ref="I77" r:id="rId13"/>
-    <hyperlink ref="I10" r:id="rId14"/>
-    <hyperlink ref="I86" r:id="rId15"/>
-    <hyperlink ref="I98" r:id="rId16"/>
+    <hyperlink ref="I39" r:id="rId2"/>
+    <hyperlink ref="I40" r:id="rId3"/>
+    <hyperlink ref="I41" r:id="rId4"/>
+    <hyperlink ref="I45" r:id="rId5"/>
+    <hyperlink ref="I47" r:id="rId6"/>
+    <hyperlink ref="I48" r:id="rId7"/>
+    <hyperlink ref="I54" r:id="rId8"/>
+    <hyperlink ref="I55" r:id="rId9"/>
+    <hyperlink ref="I64" r:id="rId10"/>
+    <hyperlink ref="I73" r:id="rId11"/>
+    <hyperlink ref="I77" r:id="rId12"/>
+    <hyperlink ref="I10" r:id="rId13"/>
+    <hyperlink ref="I86" r:id="rId14"/>
+    <hyperlink ref="I98" r:id="rId15"/>
+    <hyperlink ref="I25" r:id="rId16"/>
+    <hyperlink ref="I31" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TestCase execution done git add .
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="435">
   <si>
     <t>Product Name</t>
   </si>
@@ -1410,6 +1410,68 @@
   </si>
   <si>
     <t>visible</t>
+  </si>
+  <si>
+    <t>1. Click on 'Profile photo'
+2. Disconnect internet
+3. Click on 'Logout' button</t>
+  </si>
+  <si>
+    <t>User should not logout</t>
+  </si>
+  <si>
+    <t>working properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on 'Profile photo'
+2. Close the browser
+3. reopen the browser and website </t>
+  </si>
+  <si>
+    <t>User should be logged out from all the tab and not accessible before login again</t>
+  </si>
+  <si>
+    <t>1. open new tab on the same browser
+2. click on 'Logout' from any tab
+3. try to browse website</t>
+  </si>
+  <si>
+    <t>User should be logged out .</t>
+  </si>
+  <si>
+    <t>Test Case passed ! But I think, we have to need more improve the UI part to give user better experience.</t>
+  </si>
+  <si>
+    <t>1. Login to the website
+2. Looking for Search box for whole website.</t>
+  </si>
+  <si>
+    <t>User should be find a main search box from which user can search any valid thing.</t>
+  </si>
+  <si>
+    <t>Not found !!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think we need a main Search Box. </t>
+  </si>
+  <si>
+    <t>Should be display proper placeholder or field name for all the fields.</t>
+  </si>
+  <si>
+    <t>TC_SP_093</t>
+  </si>
+  <si>
+    <t>Check that all the links in the Footer section of the webpage is working properly or not.</t>
+  </si>
+  <si>
+    <t>1. Login to the website
+2. Click on all the links in the Footer area.</t>
+  </si>
+  <si>
+    <t>All the links (Facebook, Instragram, Youtube, LinkedIn, Google play store) should be navigate to the right pages.</t>
+  </si>
+  <si>
+    <t>Working good</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1625,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1657,6 +1719,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1800,7 +1868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1965,6 +2033,19 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2321,7 +2402,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2329,10 +2410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" topLeftCell="E121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4785,11 +4866,21 @@
       <c r="B112" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
+      <c r="C112" s="41" t="s">
+        <v>417</v>
+      </c>
+      <c r="D112" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E112" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="F112" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="G112" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H112" s="27"/>
       <c r="I112" s="27"/>
     </row>
@@ -4800,11 +4891,21 @@
       <c r="B113" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
+      <c r="C113" s="41" t="s">
+        <v>420</v>
+      </c>
+      <c r="D113" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E113" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="F113" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="G113" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H113" s="27"/>
       <c r="I113" s="27"/>
     </row>
@@ -4816,10 +4917,16 @@
         <v>217</v>
       </c>
       <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
+      <c r="D114" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="27"/>
+      <c r="F114" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="G114" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H114" s="27"/>
       <c r="I114" s="27"/>
     </row>
@@ -4830,11 +4937,21 @@
       <c r="B115" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="C115" s="27"/>
-      <c r="D115" s="27"/>
-      <c r="E115" s="27"/>
-      <c r="F115" s="27"/>
-      <c r="G115" s="27"/>
+      <c r="C115" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="D115" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E115" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="F115" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="G115" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H115" s="27"/>
       <c r="I115" s="27"/>
     </row>
@@ -4845,11 +4962,21 @@
       <c r="B116" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="C116" s="27"/>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-      <c r="F116" s="27"/>
-      <c r="G116" s="27"/>
+      <c r="C116" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E116" s="27" t="s">
+        <v>423</v>
+      </c>
+      <c r="F116" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="G116" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H116" s="27"/>
       <c r="I116" s="27"/>
     </row>
@@ -4896,12 +5023,20 @@
         <v>224</v>
       </c>
       <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
+      <c r="D120" s="25" t="s">
+        <v>241</v>
+      </c>
       <c r="E120" s="27"/>
       <c r="F120" s="27"/>
-      <c r="G120" s="27"/>
-      <c r="H120" s="27"/>
-      <c r="I120" s="27"/>
+      <c r="G120" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H120" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I120" s="64" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="121" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="25" t="s">
@@ -4910,15 +5045,27 @@
       <c r="B121" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="C121" s="27"/>
-      <c r="D121" s="27"/>
-      <c r="E121" s="27"/>
-      <c r="F121" s="27"/>
+      <c r="C121" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="D121" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E121" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="F121" s="40" t="s">
+        <v>427</v>
+      </c>
       <c r="G121" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="H121" s="27"/>
-      <c r="I121" s="27"/>
+      <c r="H121" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="I121" s="64" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="122" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="25" t="s">
@@ -4928,35 +5075,61 @@
         <v>228</v>
       </c>
       <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
+      <c r="D122" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E122" s="26" t="s">
+        <v>429</v>
+      </c>
       <c r="F122" s="27"/>
-      <c r="G122" s="27"/>
+      <c r="G122" s="48" t="s">
+        <v>7</v>
+      </c>
       <c r="H122" s="27"/>
       <c r="I122" s="27"/>
     </row>
     <row r="123" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="25" t="s">
+      <c r="A123" s="65" t="s">
         <v>229</v>
       </c>
-      <c r="B123" s="26" t="s">
+      <c r="B123" s="66" t="s">
         <v>230</v>
       </c>
-      <c r="C123" s="27"/>
-      <c r="D123" s="27"/>
-      <c r="E123" s="27"/>
-      <c r="F123" s="27"/>
-      <c r="G123" s="27"/>
-      <c r="H123" s="27"/>
-      <c r="I123" s="27"/>
+      <c r="C123" s="67"/>
+      <c r="D123" s="67"/>
+      <c r="E123" s="67"/>
+      <c r="F123" s="67"/>
+      <c r="G123" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="H123" s="67"/>
+      <c r="I123" s="67"/>
+    </row>
+    <row r="124" spans="1:9" s="27" customFormat="1" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="28" t="s">
+        <v>430</v>
+      </c>
+      <c r="B124" s="29" t="s">
+        <v>431</v>
+      </c>
+      <c r="C124" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="D124" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="E124" s="26" t="s">
+        <v>433</v>
+      </c>
+      <c r="F124" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="G124" s="68" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A101:C101"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:B1"/>
@@ -4968,6 +5141,11 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A101:C101"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I26" r:id="rId1"/>

</xml_diff>

<commit_message>
TestCase execution result is : Total case-93, Pass-69, Fail-18, Warning-06
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="325"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="222"/>
   </bookViews>
   <sheets>
     <sheet name="Profile_Page_TestCases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="435">
   <si>
     <t>Product Name</t>
   </si>
@@ -1378,9 +1378,6 @@
     <t>Should not be updated tag name.</t>
   </si>
   <si>
-    <t>Tag name is updated.</t>
-  </si>
-  <si>
     <t>1. Click on 'Profile photo'
 2. Click on 'Students Analytics' button</t>
   </si>
@@ -1472,6 +1469,9 @@
   </si>
   <si>
     <t>Working good</t>
+  </si>
+  <si>
+    <t>Tag name is updated with only spaces.</t>
   </si>
 </sst>
 </file>
@@ -1480,14 +1480,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1624,8 +1616,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1646,37 +1645,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1725,6 +1700,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1866,72 +1847,56 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1947,93 +1912,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2043,7 +1988,48 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2402,7 +2388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2412,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2430,11 +2416,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2449,16 +2435,16 @@
       <c r="G1" s="10">
         <v>44572</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="57"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="59"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
@@ -2471,15 +2457,19 @@
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="11"/>
+      <c r="G2" s="10">
+        <v>44573</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="60">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="60"/>
-      <c r="B3" s="59"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -2493,16 +2483,18 @@
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="61">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="59"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
@@ -2518,2618 +2510,2633 @@
       <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="13"/>
+      <c r="I4" s="62">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="62" t="s">
+      <c r="B5" s="55"/>
+      <c r="C5" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="17" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:10" s="36" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+      <c r="I5" s="67">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="28" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="45" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:10" s="37" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="41" t="s">
         <v>232</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="G7" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" spans="1:10" s="27" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="G7" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="38"/>
+    </row>
+    <row r="8" spans="1:10" s="19" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="G8" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="37"/>
-    </row>
-    <row r="9" spans="1:10" s="27" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+      <c r="D8" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="1:10" s="19" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="D9" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="H9" s="51" t="s">
+      <c r="H9" s="43" t="s">
         <v>239</v>
       </c>
-      <c r="J9" s="37"/>
-    </row>
-    <row r="10" spans="1:10" s="27" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="J9" s="29"/>
+    </row>
+    <row r="10" spans="1:10" s="19" customFormat="1" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E10" s="40" t="s">
+      <c r="D10" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E10" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="43" t="s">
         <v>243</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="J10" s="37"/>
-    </row>
-    <row r="11" spans="1:10" s="27" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28" t="s">
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" s="19" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E11" s="40" t="s">
+      <c r="D11" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G11" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="37"/>
-    </row>
-    <row r="12" spans="1:10" s="27" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="G11" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:10" s="19" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12" s="40" t="s">
+      <c r="D12" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G12" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="37"/>
-    </row>
-    <row r="13" spans="1:10" s="27" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28" t="s">
+      <c r="G12" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="29"/>
+    </row>
+    <row r="13" spans="1:10" s="19" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E13" s="40" t="s">
+      <c r="D13" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G13" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" s="37"/>
-    </row>
-    <row r="14" spans="1:10" s="27" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="28" t="s">
+      <c r="G13" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="29"/>
+    </row>
+    <row r="14" spans="1:10" s="19" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E14" s="40" t="s">
+      <c r="D14" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G14" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="37"/>
-    </row>
-    <row r="15" spans="1:10" s="27" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28" t="s">
+      <c r="G14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="29"/>
+    </row>
+    <row r="15" spans="1:10" s="19" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E15" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G15" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="37"/>
-    </row>
-    <row r="16" spans="1:10" s="27" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="G15" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="29"/>
+    </row>
+    <row r="16" spans="1:10" s="19" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E16" s="40" t="s">
+      <c r="D16" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="G16" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" s="37"/>
-    </row>
-    <row r="17" spans="1:10" s="31" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="61" t="s">
+      <c r="G16" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="38"/>
-    </row>
-    <row r="18" spans="1:10" s="27" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="28" t="s">
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="30"/>
+    </row>
+    <row r="18" spans="1:10" s="19" customFormat="1" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E18" s="40" t="s">
+      <c r="D18" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E18" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="32" t="s">
         <v>247</v>
       </c>
-      <c r="G18" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="37"/>
-    </row>
-    <row r="19" spans="1:10" s="27" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28" t="s">
+      <c r="G18" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" s="19" customFormat="1" ht="80.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="D19" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="G19" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="37"/>
-    </row>
-    <row r="20" spans="1:10" s="27" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
+      <c r="G19" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="29"/>
+    </row>
+    <row r="20" spans="1:10" s="19" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D20" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E20" s="26" t="s">
+      <c r="D20" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="G20" s="52" t="s">
+      <c r="G20" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="J20" s="37"/>
-    </row>
-    <row r="21" spans="1:10" s="27" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
+      <c r="J20" s="29"/>
+    </row>
+    <row r="21" spans="1:10" s="19" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E21" s="40" t="s">
+      <c r="D21" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E21" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="G21" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" s="37"/>
-    </row>
-    <row r="22" spans="1:10" s="27" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28" t="s">
+      <c r="G21" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:10" s="19" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="D22" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E22" s="26" t="s">
+      <c r="D22" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="G22" s="50" t="s">
+      <c r="G22" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="53" t="s">
+      <c r="H22" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="1:10" s="27" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:10" s="19" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="D23" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E23" s="40" t="s">
+      <c r="D23" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E23" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="G23" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="1:10" s="27" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+      <c r="G23" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="1:10" s="19" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E24" s="26" t="s">
+      <c r="D24" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="G24" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J24" s="37"/>
-    </row>
-    <row r="25" spans="1:10" s="27" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="G24" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="29"/>
+    </row>
+    <row r="25" spans="1:10" s="19" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="H25" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="J25" s="37"/>
-    </row>
-    <row r="26" spans="1:10" s="27" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+      <c r="J25" s="29"/>
+    </row>
+    <row r="26" spans="1:10" s="19" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="37"/>
-    </row>
-    <row r="27" spans="1:10" s="27" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" s="19" customFormat="1" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="D27" s="55" t="s">
+      <c r="D27" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="32" t="s">
         <v>279</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="32" t="s">
         <v>280</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="53" t="s">
+      <c r="H27" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="J27" s="37"/>
-    </row>
-    <row r="28" spans="1:10" s="27" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" s="19" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="32" t="s">
         <v>283</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="G28" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J28" s="37"/>
-    </row>
-    <row r="29" spans="1:10" s="27" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="G28" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="1:10" s="19" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="G29" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J29" s="37"/>
-    </row>
-    <row r="30" spans="1:10" s="27" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
+      <c r="G29" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" s="19" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="37"/>
-    </row>
-    <row r="31" spans="1:10" s="27" customFormat="1" ht="107.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28" t="s">
+      <c r="G30" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" s="19" customFormat="1" ht="107.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="18" t="s">
         <v>288</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="32" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="53" t="s">
+      <c r="H31" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="J31" s="37"/>
-    </row>
-    <row r="32" spans="1:10" s="27" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="28" t="s">
+      <c r="J31" s="29"/>
+    </row>
+    <row r="32" spans="1:10" s="19" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="G32" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J32" s="37"/>
+      <c r="G32" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="29"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-    </row>
-    <row r="35" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="56" t="s">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
     </row>
     <row r="36" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="D36" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E36" s="40" t="s">
+      <c r="D36" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E36" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" s="32" t="s">
         <v>298</v>
       </c>
-      <c r="G36" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
+      <c r="G36" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
     </row>
     <row r="37" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E37" s="27" t="s">
+      <c r="C37" s="19"/>
+      <c r="D37" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="F37" s="27" t="s">
+      <c r="F37" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="G37" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
+      <c r="G37" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E38" s="26" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="G38" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
+      <c r="G38" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
     </row>
     <row r="39" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="32" t="s">
         <v>305</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H39" s="27"/>
-      <c r="I39" s="33" t="s">
+      <c r="H39" s="19"/>
+      <c r="I39" s="25" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="32" t="s">
         <v>310</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="G40" s="50" t="s">
+      <c r="G40" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H40" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="25" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="D41" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E41" s="40" t="s">
+      <c r="D41" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E41" s="32" t="s">
         <v>313</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="G41" s="32" t="s">
+      <c r="G41" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H41" s="53" t="s">
+      <c r="H41" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I41" s="33" t="s">
+      <c r="I41" s="25" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-    </row>
-    <row r="44" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="56" t="s">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
     </row>
     <row r="45" spans="1:9" ht="91" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="D45" s="54" t="s">
+      <c r="D45" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="E45" s="40" t="s">
+      <c r="E45" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="F45" s="40" t="s">
+      <c r="F45" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G45" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H45" s="53" t="s">
+      <c r="H45" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I45" s="33" t="s">
+      <c r="I45" s="25" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F46" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="G46" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
+      <c r="G46" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:9" ht="91" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="F47" s="32" t="s">
         <v>325</v>
       </c>
-      <c r="G47" s="32" t="s">
+      <c r="G47" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H47" s="53" t="s">
+      <c r="H47" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I47" s="33" t="s">
+      <c r="I47" s="25" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="C48" s="41" t="s">
+      <c r="C48" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="D48" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E48" s="26" t="s">
+      <c r="D48" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="F48" s="25" t="s">
+      <c r="F48" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="G48" s="32" t="s">
+      <c r="G48" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H48" s="53" t="s">
+      <c r="H48" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I48" s="33" t="s">
+      <c r="I48" s="25" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C49" s="41" t="s">
+      <c r="C49" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="E49" s="40" t="s">
+      <c r="E49" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="F49" s="40" t="s">
+      <c r="F49" s="32" t="s">
         <v>332</v>
       </c>
-      <c r="G49" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
+      <c r="G49" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
     </row>
     <row r="50" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
     </row>
     <row r="51" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="D51" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E51" s="26" t="s">
+      <c r="D51" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="G51" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
+      <c r="G51" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
     </row>
     <row r="52" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="41" t="s">
+      <c r="C52" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="D52" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E52" s="40" t="s">
+      <c r="D52" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E52" s="32" t="s">
         <v>338</v>
       </c>
-      <c r="F52" s="26" t="s">
+      <c r="F52" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="G52" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
+      <c r="G52" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
     </row>
     <row r="53" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="D53" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E53" s="26" t="s">
+      <c r="D53" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>340</v>
       </c>
-      <c r="F53" s="40" t="s">
+      <c r="F53" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="G53" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
+      <c r="G53" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
     </row>
     <row r="54" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="E54" s="40" t="s">
+      <c r="E54" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="G54" s="32" t="s">
+      <c r="G54" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H54" s="53" t="s">
+      <c r="H54" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I54" s="33" t="s">
+      <c r="I54" s="25" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="32" t="s">
         <v>343</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="32" t="s">
         <v>346</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="32" t="s">
         <v>347</v>
       </c>
-      <c r="G55" s="32" t="s">
+      <c r="G55" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H55" s="53" t="s">
+      <c r="H55" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I55" s="33" t="s">
+      <c r="I55" s="25" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="99.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="40" t="s">
+      <c r="D56" s="19"/>
+      <c r="E56" s="32" t="s">
         <v>350</v>
       </c>
-      <c r="F56" s="26" t="s">
+      <c r="F56" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="G56" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
+      <c r="G56" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-    </row>
-    <row r="59" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="56" t="s">
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+    </row>
+    <row r="59" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="56"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
     </row>
     <row r="60" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="25" t="s">
+      <c r="A60" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C60" s="40" t="s">
+      <c r="C60" s="32" t="s">
         <v>352</v>
       </c>
-      <c r="D60" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E60" s="40" t="s">
+      <c r="D60" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E60" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="F60" s="40" t="s">
+      <c r="F60" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="G60" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
+      <c r="G60" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
     </row>
     <row r="61" spans="1:9" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="25" t="s">
+      <c r="A61" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="18" t="s">
         <v>355</v>
       </c>
-      <c r="D61" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E61" s="40" t="s">
+      <c r="D61" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E61" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="F61" s="40" t="s">
+      <c r="F61" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="G61" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
+      <c r="G61" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
     </row>
     <row r="62" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="26" t="s">
+      <c r="C62" s="18" t="s">
         <v>356</v>
       </c>
-      <c r="D62" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E62" s="40" t="s">
+      <c r="D62" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E62" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="F62" s="40" t="s">
+      <c r="F62" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="G62" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
+      <c r="G62" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="25" t="s">
+      <c r="A63" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="26" t="s">
+      <c r="B63" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E63" s="40" t="s">
+      <c r="C63" s="19"/>
+      <c r="D63" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="F63" s="40" t="s">
+      <c r="F63" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="G63" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H63" s="27"/>
-      <c r="I63" s="27"/>
+      <c r="G63" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C64" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="D64" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E64" s="26" t="s">
+      <c r="D64" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E64" s="18" t="s">
         <v>358</v>
       </c>
-      <c r="F64" s="40" t="s">
+      <c r="F64" s="32" t="s">
         <v>359</v>
       </c>
-      <c r="G64" s="32" t="s">
+      <c r="G64" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H64" s="53" t="s">
+      <c r="H64" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I64" s="33" t="s">
+      <c r="I64" s="25" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C65" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D65" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E65" s="27" t="s">
+      <c r="D65" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E65" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="F65" s="27" t="s">
+      <c r="F65" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="G65" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
+      <c r="G65" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
     </row>
     <row r="66" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D66" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H66" s="27"/>
-      <c r="I66" s="27"/>
+      <c r="D66" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C67" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D67" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
+      <c r="D67" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
     </row>
     <row r="68" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="26" t="s">
+      <c r="C68" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D68" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H68" s="27"/>
-      <c r="I68" s="27"/>
+      <c r="D68" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
     </row>
     <row r="69" spans="1:9" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="25" t="s">
+      <c r="A69" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D69" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
+      <c r="D69" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
     </row>
     <row r="70" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B70" s="26" t="s">
+      <c r="B70" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D70" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
+      <c r="D70" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
     </row>
     <row r="71" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="26" t="s">
+      <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C71" s="26" t="s">
+      <c r="C71" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D71" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
+      <c r="D71" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
     </row>
     <row r="72" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="25" t="s">
+      <c r="A72" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="26" t="s">
+      <c r="B72" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C72" s="26" t="s">
+      <c r="C72" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D72" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
+      <c r="D72" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
     </row>
     <row r="73" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="25" t="s">
+      <c r="A73" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B73" s="26" t="s">
+      <c r="B73" s="18" t="s">
         <v>363</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="D73" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E73" s="26" t="s">
+      <c r="D73" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="F73" s="26" t="s">
+      <c r="F73" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="G73" s="32" t="s">
+      <c r="G73" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H73" s="53" t="s">
+      <c r="H73" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="I73" s="33" t="s">
+      <c r="I73" s="25" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B74" s="26" t="s">
+      <c r="B74" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="26" t="s">
+      <c r="C74" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="D74" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E74" s="26" t="s">
+      <c r="D74" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E74" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="F74" s="40" t="s">
+      <c r="F74" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="G74" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H74" s="27"/>
-      <c r="I74" s="27"/>
+      <c r="G74" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
     </row>
     <row r="75" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="25" t="s">
+      <c r="A75" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="C75" s="26" t="s">
+      <c r="C75" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="D75" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E75" s="40" t="s">
+      <c r="D75" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E75" s="32" t="s">
         <v>370</v>
       </c>
-      <c r="F75" s="40" t="s">
+      <c r="F75" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="G75" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
+      <c r="G75" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
     </row>
     <row r="76" spans="1:9" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="25" t="s">
+      <c r="A76" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="26" t="s">
+      <c r="B76" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="27"/>
-      <c r="D76" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E76" s="26" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E76" s="18" t="s">
         <v>371</v>
       </c>
-      <c r="F76" s="40" t="s">
+      <c r="F76" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="G76" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
+      <c r="G76" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
     </row>
     <row r="77" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="26" t="s">
+      <c r="B77" s="18" t="s">
         <v>372</v>
       </c>
-      <c r="C77" s="26" t="s">
+      <c r="C77" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="D77" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E77" s="40" t="s">
+      <c r="D77" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E77" s="32" t="s">
         <v>374</v>
       </c>
-      <c r="F77" s="26" t="s">
+      <c r="F77" s="18" t="s">
         <v>375</v>
       </c>
-      <c r="G77" s="35" t="s">
+      <c r="G77" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="H77" s="53" t="s">
+      <c r="H77" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I77" s="33" t="s">
+      <c r="I77" s="25" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="B78" s="26" t="s">
+      <c r="B78" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C78" s="41" t="s">
+      <c r="C78" s="33" t="s">
         <v>376</v>
       </c>
-      <c r="D78" s="40" t="s">
+      <c r="D78" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="E78" s="40" t="s">
+      <c r="E78" s="32" t="s">
         <v>378</v>
       </c>
-      <c r="F78" s="40" t="s">
+      <c r="F78" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G78" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
+      <c r="G78" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
     </row>
     <row r="79" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="25" t="s">
+      <c r="A79" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="C79" s="27"/>
-      <c r="D79" s="40" t="s">
+      <c r="C79" s="19"/>
+      <c r="D79" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="32" t="s">
         <v>381</v>
       </c>
-      <c r="F79" s="40"/>
-      <c r="G79" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
+      <c r="F79" s="32"/>
+      <c r="G79" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
     </row>
     <row r="80" spans="1:9" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="25" t="s">
+      <c r="A80" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B80" s="26" t="s">
+      <c r="B80" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="C80" s="26" t="s">
+      <c r="C80" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="D80" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E80" s="40" t="s">
+      <c r="D80" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E80" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="F80" s="40" t="s">
+      <c r="F80" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G80" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
+      <c r="G80" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
     </row>
     <row r="81" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="25" t="s">
+      <c r="A81" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C81" s="26" t="s">
+      <c r="C81" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="D81" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E81" s="27" t="s">
+      <c r="D81" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E81" s="19" t="s">
         <v>385</v>
       </c>
-      <c r="F81" s="40" t="s">
+      <c r="F81" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G81" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
+      <c r="G81" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="27"/>
-      <c r="I83" s="27"/>
-    </row>
-    <row r="84" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="56" t="s">
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+    </row>
+    <row r="84" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="B84" s="56"/>
-      <c r="C84" s="56"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="39"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="39"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="53"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="31"/>
+      <c r="I84" s="31"/>
     </row>
     <row r="85" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="B85" s="26" t="s">
+      <c r="B85" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="C85" s="41" t="s">
+      <c r="C85" s="33" t="s">
         <v>386</v>
       </c>
-      <c r="D85" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E85" s="40" t="s">
+      <c r="D85" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E85" s="32" t="s">
         <v>387</v>
       </c>
-      <c r="F85" s="40" t="s">
+      <c r="F85" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G85" s="27"/>
-      <c r="H85" s="27"/>
-      <c r="I85" s="27"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+      <c r="I85" s="19"/>
     </row>
     <row r="86" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="B86" s="26" t="s">
+      <c r="B86" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="41" t="s">
+      <c r="C86" s="33" t="s">
         <v>386</v>
       </c>
-      <c r="D86" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E86" s="40" t="s">
+      <c r="D86" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E86" s="32" t="s">
         <v>388</v>
       </c>
-      <c r="F86" s="40" t="s">
+      <c r="F86" s="32" t="s">
         <v>389</v>
       </c>
-      <c r="G86" s="32" t="s">
+      <c r="G86" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H86" s="53" t="s">
+      <c r="H86" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I86" s="33" t="s">
+      <c r="I86" s="25" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="74.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="25" t="s">
+      <c r="A87" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B87" s="26" t="s">
+      <c r="B87" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="C87" s="26" t="s">
+      <c r="C87" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D87" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E87" s="26" t="s">
+      <c r="D87" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E87" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="F87" s="40" t="s">
+      <c r="F87" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G87" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H87" s="27"/>
-      <c r="I87" s="27"/>
+      <c r="G87" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
     </row>
     <row r="88" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="25" t="s">
+      <c r="A88" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B88" s="26" t="s">
+      <c r="B88" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C88" s="41" t="s">
+      <c r="C88" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="D88" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E88" s="26" t="s">
+      <c r="D88" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E88" s="18" t="s">
         <v>391</v>
       </c>
-      <c r="F88" s="40" t="s">
+      <c r="F88" s="32" t="s">
         <v>392</v>
       </c>
-      <c r="G88" s="32" t="s">
+      <c r="G88" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H88" s="53" t="s">
+      <c r="H88" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I88" s="27"/>
+      <c r="I88" s="19"/>
     </row>
     <row r="89" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="25" t="s">
+      <c r="A89" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="B89" s="26" t="s">
+      <c r="B89" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C89" s="27"/>
-      <c r="D89" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E89" s="27" t="s">
+      <c r="C89" s="19"/>
+      <c r="D89" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E89" s="32" t="s">
         <v>393</v>
       </c>
-      <c r="F89" s="27" t="s">
+      <c r="F89" s="32" t="s">
         <v>379</v>
       </c>
-      <c r="G89" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
+      <c r="G89" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="25" t="s">
+      <c r="A90" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B90" s="26" t="s">
+      <c r="B90" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="C90" s="41" t="s">
+      <c r="C90" s="33" t="s">
         <v>394</v>
       </c>
-      <c r="D90" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E90" s="41" t="s">
+      <c r="D90" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E90" s="18" t="s">
         <v>395</v>
       </c>
-      <c r="F90" s="27" t="s">
+      <c r="F90" s="32" t="s">
         <v>396</v>
       </c>
-      <c r="G90" s="42" t="s">
+      <c r="G90" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="H90" s="53" t="s">
+      <c r="H90" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="I90" s="27"/>
+      <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A91" s="27"/>
-      <c r="B91" s="27"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="27"/>
-      <c r="I91" s="27"/>
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A92" s="27"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27"/>
-      <c r="H92" s="27"/>
-      <c r="I92" s="27"/>
-    </row>
-    <row r="93" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="56" t="s">
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
+    </row>
+    <row r="93" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="B93" s="56"/>
-      <c r="C93" s="56"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="39"/>
+      <c r="B93" s="53"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="31"/>
+      <c r="E93" s="31"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="31"/>
+      <c r="I93" s="31"/>
     </row>
     <row r="94" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="25" t="s">
+      <c r="A94" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B94" s="26" t="s">
+      <c r="B94" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C94" s="41" t="s">
+      <c r="C94" s="33" t="s">
         <v>245</v>
       </c>
-      <c r="D94" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E94" s="27"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H94" s="27"/>
-      <c r="I94" s="27"/>
+      <c r="D94" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
     </row>
     <row r="95" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="25" t="s">
+      <c r="A95" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="26" t="s">
+      <c r="B95" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="C95" s="26" t="s">
+      <c r="C95" s="18" t="s">
         <v>397</v>
       </c>
-      <c r="D95" s="25" t="s">
+      <c r="D95" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="E95" s="40" t="s">
+      <c r="E95" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="F95" s="40" t="s">
+      <c r="F95" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="G95" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H95" s="27"/>
-      <c r="I95" s="27"/>
+      <c r="G95" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="B96" s="26" t="s">
+      <c r="B96" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="C96" s="26" t="s">
+      <c r="C96" s="18" t="s">
         <v>401</v>
       </c>
-      <c r="D96" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E96" s="40" t="s">
+      <c r="D96" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E96" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="F96" s="40" t="s">
+      <c r="F96" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="G96" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H96" s="27"/>
-      <c r="I96" s="27"/>
+      <c r="G96" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="25" t="s">
+      <c r="A97" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="26" t="s">
+      <c r="B97" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C97" s="26" t="s">
+      <c r="C97" s="18" t="s">
         <v>402</v>
       </c>
-      <c r="D97" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E97" s="40" t="s">
+      <c r="D97" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E97" s="32" t="s">
         <v>403</v>
       </c>
-      <c r="F97" s="40" t="s">
+      <c r="F97" s="32" t="s">
         <v>400</v>
       </c>
-      <c r="G97" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H97" s="27"/>
-      <c r="I97" s="27"/>
+      <c r="G97" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="25" t="s">
+      <c r="A98" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="26" t="s">
+      <c r="B98" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="C98" s="26" t="s">
+      <c r="C98" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="D98" s="25" t="s">
+      <c r="D98" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="E98" s="40" t="s">
+      <c r="E98" s="32" t="s">
         <v>406</v>
       </c>
-      <c r="F98" s="40" t="s">
+      <c r="F98" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="G98" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H98" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="I98" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="19"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="19"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" s="19"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+    </row>
+    <row r="101" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="B101" s="53"/>
+      <c r="C101" s="53"/>
+      <c r="D101" s="31"/>
+      <c r="E101" s="31"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="31"/>
+      <c r="I101" s="31"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" s="19"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+    </row>
+    <row r="103" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" s="33" t="s">
         <v>407</v>
       </c>
-      <c r="G98" s="32" t="s">
+      <c r="D103" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E103" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="F103" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="G103" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+    </row>
+    <row r="104" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="D104" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="F104" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="G104" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+    </row>
+    <row r="105" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E105" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="F105" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="G105" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H105" s="19"/>
+      <c r="I105" s="19"/>
+    </row>
+    <row r="106" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="D106" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E106" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="F106" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="G106" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+    </row>
+    <row r="107" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C107" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="D107" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E107" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="F107" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="G107" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" s="19"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+    </row>
+    <row r="110" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="B110" s="53"/>
+      <c r="C110" s="53"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="31"/>
+      <c r="F110" s="31"/>
+      <c r="G110" s="31"/>
+      <c r="H110" s="31"/>
+      <c r="I110" s="31"/>
+    </row>
+    <row r="111" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="F111" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="G111" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H111" s="19"/>
+      <c r="I111" s="19"/>
+    </row>
+    <row r="112" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C112" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="F112" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G112" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+    </row>
+    <row r="113" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="C113" s="33" t="s">
+        <v>419</v>
+      </c>
+      <c r="D113" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E113" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="F113" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G113" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
+    </row>
+    <row r="114" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B114" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="C114" s="19"/>
+      <c r="D114" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G114" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" s="19"/>
+      <c r="I114" s="19"/>
+    </row>
+    <row r="115" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B115" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="D115" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G115" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H115" s="19"/>
+      <c r="I115" s="19"/>
+    </row>
+    <row r="116" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B116" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="C116" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="F116" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G116" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" s="19"/>
+      <c r="I116" s="19"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="19"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="19"/>
+      <c r="I117" s="19"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19"/>
+      <c r="I118" s="19"/>
+    </row>
+    <row r="119" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="B119" s="53"/>
+      <c r="C119" s="53"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="31"/>
+      <c r="F119" s="31"/>
+      <c r="G119" s="31"/>
+      <c r="H119" s="31"/>
+      <c r="I119" s="31"/>
+    </row>
+    <row r="120" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B120" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C120" s="19"/>
+      <c r="D120" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H120" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="I120" s="48" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="D121" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E121" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="F121" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="G121" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H98" s="53" t="s">
-        <v>243</v>
-      </c>
-      <c r="I98" s="33" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="27"/>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="27"/>
-      <c r="B100" s="27"/>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="27"/>
-      <c r="I100" s="27"/>
-    </row>
-    <row r="101" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="56" t="s">
-        <v>197</v>
-      </c>
-      <c r="B101" s="56"/>
-      <c r="C101" s="56"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="39"/>
-      <c r="G101" s="39"/>
-      <c r="H101" s="39"/>
-      <c r="I101" s="39"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A102" s="27"/>
-      <c r="B102" s="27"/>
-      <c r="C102" s="27"/>
-      <c r="D102" s="27"/>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
-    </row>
-    <row r="103" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B103" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="C103" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="D103" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E103" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="F103" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="G103" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H103" s="27"/>
-      <c r="I103" s="27"/>
-    </row>
-    <row r="104" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="25" t="s">
-        <v>200</v>
-      </c>
-      <c r="B104" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="C104" s="41" t="s">
-        <v>408</v>
-      </c>
-      <c r="D104" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>411</v>
-      </c>
-      <c r="F104" s="27" t="s">
-        <v>400</v>
-      </c>
-      <c r="G104" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H104" s="27"/>
-      <c r="I104" s="27"/>
-    </row>
-    <row r="105" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="B105" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="C105" s="41" t="s">
-        <v>412</v>
-      </c>
-      <c r="D105" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E105" s="27" t="s">
-        <v>413</v>
-      </c>
-      <c r="F105" s="27" t="s">
-        <v>400</v>
-      </c>
-      <c r="G105" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H105" s="27"/>
-      <c r="I105" s="27"/>
-    </row>
-    <row r="106" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="B106" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="C106" s="41" t="s">
-        <v>414</v>
-      </c>
-      <c r="D106" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E106" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="F106" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="G106" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H106" s="27"/>
-      <c r="I106" s="27"/>
-    </row>
-    <row r="107" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="B107" s="26" t="s">
-        <v>207</v>
-      </c>
-      <c r="C107" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="D107" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E107" s="27" t="s">
-        <v>409</v>
-      </c>
-      <c r="F107" s="27" t="s">
-        <v>410</v>
-      </c>
-      <c r="G107" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A108" s="27"/>
-      <c r="B108" s="27"/>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="27"/>
-      <c r="I108" s="27"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A109" s="27"/>
-      <c r="B109" s="27"/>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="27"/>
-      <c r="F109" s="27"/>
-      <c r="G109" s="27"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="27"/>
-    </row>
-    <row r="110" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="56" t="s">
-        <v>209</v>
-      </c>
-      <c r="B110" s="56"/>
-      <c r="C110" s="56"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="39"/>
-      <c r="F110" s="39"/>
-      <c r="G110" s="39"/>
-      <c r="H110" s="39"/>
-      <c r="I110" s="39"/>
-    </row>
-    <row r="111" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="B111" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="C111" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="D111" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E111" s="27" t="s">
-        <v>415</v>
-      </c>
-      <c r="F111" s="27" t="s">
-        <v>416</v>
-      </c>
-      <c r="G111" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-    </row>
-    <row r="112" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="B112" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="C112" s="41" t="s">
-        <v>417</v>
-      </c>
-      <c r="D112" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E112" s="27" t="s">
-        <v>418</v>
-      </c>
-      <c r="F112" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="G112" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-    </row>
-    <row r="113" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="B113" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="C113" s="41" t="s">
-        <v>420</v>
-      </c>
-      <c r="D113" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E113" s="27" t="s">
-        <v>418</v>
-      </c>
-      <c r="F113" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="G113" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-    </row>
-    <row r="114" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="B114" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="C114" s="27"/>
-      <c r="D114" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="G114" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
-    </row>
-    <row r="115" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="B115" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="C115" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="D115" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>421</v>
-      </c>
-      <c r="F115" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="G115" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H115" s="27"/>
-      <c r="I115" s="27"/>
-    </row>
-    <row r="116" spans="1:9" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="B116" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="C116" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="D116" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E116" s="27" t="s">
-        <v>423</v>
-      </c>
-      <c r="F116" s="27" t="s">
-        <v>419</v>
-      </c>
-      <c r="G116" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H116" s="27"/>
-      <c r="I116" s="27"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A117" s="27"/>
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="27"/>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A118" s="27"/>
-      <c r="B118" s="27"/>
-      <c r="C118" s="27"/>
-      <c r="D118" s="27"/>
-      <c r="E118" s="27"/>
-      <c r="F118" s="27"/>
-      <c r="G118" s="27"/>
-      <c r="H118" s="27"/>
-      <c r="I118" s="27"/>
-    </row>
-    <row r="119" spans="1:9" s="30" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A119" s="56" t="s">
-        <v>222</v>
-      </c>
-      <c r="B119" s="56"/>
-      <c r="C119" s="56"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="39"/>
-      <c r="H119" s="39"/>
-      <c r="I119" s="39"/>
-    </row>
-    <row r="120" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="B120" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="C120" s="27"/>
-      <c r="D120" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H120" s="53" t="s">
+      <c r="H121" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="I120" s="64" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="25" t="s">
-        <v>225</v>
-      </c>
-      <c r="B121" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="C121" s="26" t="s">
-        <v>425</v>
-      </c>
-      <c r="D121" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E121" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="F121" s="40" t="s">
+      <c r="I121" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="G121" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="H121" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="I121" s="64" t="s">
+    </row>
+    <row r="122" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="C122" s="19"/>
+      <c r="D122" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E122" s="18" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="B122" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="C122" s="27"/>
-      <c r="D122" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E122" s="26" t="s">
+      <c r="F122" s="19"/>
+      <c r="G122" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H122" s="19"/>
+      <c r="I122" s="19"/>
+    </row>
+    <row r="123" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="49" t="s">
+        <v>229</v>
+      </c>
+      <c r="B123" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="C123" s="51"/>
+      <c r="D123" s="51"/>
+      <c r="E123" s="51"/>
+      <c r="F123" s="51"/>
+      <c r="G123" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H123" s="51"/>
+      <c r="I123" s="51"/>
+    </row>
+    <row r="124" spans="1:9" s="19" customFormat="1" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="F122" s="27"/>
-      <c r="G122" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H122" s="27"/>
-      <c r="I122" s="27"/>
-    </row>
-    <row r="123" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="65" t="s">
-        <v>229</v>
-      </c>
-      <c r="B123" s="66" t="s">
-        <v>230</v>
-      </c>
-      <c r="C123" s="67"/>
-      <c r="D123" s="67"/>
-      <c r="E123" s="67"/>
-      <c r="F123" s="67"/>
-      <c r="G123" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="H123" s="67"/>
-      <c r="I123" s="67"/>
-    </row>
-    <row r="124" spans="1:9" s="27" customFormat="1" ht="69.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="28" t="s">
+      <c r="B124" s="21" t="s">
         <v>430</v>
       </c>
-      <c r="B124" s="29" t="s">
+      <c r="C124" s="18" t="s">
         <v>431</v>
       </c>
-      <c r="C124" s="26" t="s">
+      <c r="D124" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E124" s="18" t="s">
         <v>432</v>
       </c>
-      <c r="D124" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="E124" s="26" t="s">
+      <c r="F124" s="32" t="s">
         <v>433</v>
       </c>
-      <c r="F124" s="40" t="s">
-        <v>434</v>
-      </c>
-      <c r="G124" s="68" t="s">
+      <c r="G124" s="52" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A101:C101"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:B1"/>
@@ -5141,11 +5148,6 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A101:C101"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I26" r:id="rId1"/>

</xml_diff>

<commit_message>
add the final report
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1991,8 +1991,32 @@
     <xf numFmtId="0" fontId="14" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2008,30 +2032,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2388,7 +2388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2416,10 +2416,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="11" t="s">
         <v>27</v>
       </c>
@@ -2435,16 +2435,16 @@
       <c r="G1" s="10">
         <v>44572</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="66"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
@@ -2460,16 +2460,16 @@
       <c r="G2" s="10">
         <v>44573</v>
       </c>
-      <c r="H2" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="60">
+      <c r="H2" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="53">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
-      <c r="B3" s="55"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -2483,18 +2483,18 @@
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="61">
+      <c r="I3" s="54">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="34" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="55"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
@@ -2510,29 +2510,29 @@
       <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="62">
+      <c r="I4" s="55">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="58" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="63" t="s">
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="59">
         <v>93</v>
       </c>
     </row>
@@ -2809,11 +2809,11 @@
       <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="65" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
@@ -3205,11 +3205,11 @@
       <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
       <c r="F35" s="31"/>
@@ -3396,11 +3396,11 @@
       <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="53" t="s">
+      <c r="A44" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
       <c r="F44" s="31"/>
@@ -3743,11 +3743,11 @@
       <c r="I58" s="19"/>
     </row>
     <row r="59" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="53" t="s">
+      <c r="A59" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
       <c r="D59" s="31"/>
       <c r="E59" s="31"/>
       <c r="F59" s="31"/>
@@ -4304,11 +4304,11 @@
       <c r="I83" s="19"/>
     </row>
     <row r="84" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="53" t="s">
+      <c r="A84" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="B84" s="53"/>
-      <c r="C84" s="53"/>
+      <c r="B84" s="60"/>
+      <c r="C84" s="60"/>
       <c r="D84" s="31"/>
       <c r="E84" s="31"/>
       <c r="F84" s="31"/>
@@ -4493,11 +4493,11 @@
       <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="53" t="s">
+      <c r="A93" s="60" t="s">
         <v>185</v>
       </c>
-      <c r="B93" s="53"/>
-      <c r="C93" s="53"/>
+      <c r="B93" s="60"/>
+      <c r="C93" s="60"/>
       <c r="D93" s="31"/>
       <c r="E93" s="31"/>
       <c r="F93" s="31"/>
@@ -4653,11 +4653,11 @@
       <c r="I100" s="19"/>
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="53" t="s">
+      <c r="A101" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="B101" s="53"/>
-      <c r="C101" s="53"/>
+      <c r="B101" s="60"/>
+      <c r="C101" s="60"/>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
       <c r="F101" s="31"/>
@@ -4824,11 +4824,11 @@
       <c r="I109" s="19"/>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="53" t="s">
+      <c r="A110" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="B110" s="53"/>
-      <c r="C110" s="53"/>
+      <c r="B110" s="60"/>
+      <c r="C110" s="60"/>
       <c r="D110" s="31"/>
       <c r="E110" s="31"/>
       <c r="F110" s="31"/>
@@ -5005,11 +5005,11 @@
       <c r="I118" s="19"/>
     </row>
     <row r="119" spans="1:9" s="22" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A119" s="53" t="s">
+      <c r="A119" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="B119" s="53"/>
-      <c r="C119" s="53"/>
+      <c r="B119" s="60"/>
+      <c r="C119" s="60"/>
       <c r="D119" s="31"/>
       <c r="E119" s="31"/>
       <c r="F119" s="31"/>
@@ -5132,11 +5132,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A110:C110"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A84:C84"/>
-    <mergeCell ref="A93:C93"/>
-    <mergeCell ref="A101:C101"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:B1"/>
@@ -5148,6 +5143,11 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A110:C110"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A101:C101"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I26" r:id="rId1"/>

</xml_diff>